<commit_message>
work on chambers/white and Luk hook scripts
</commit_message>
<xml_diff>
--- a/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
+++ b/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Chambers_et_al_2019/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543DD21B-9705-F142-A2A5-B8546854C9F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453DC003-EBA9-0548-9D7A-039E3D6C7A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25740" yWindow="460" windowWidth="38260" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
@@ -259,12 +259,6 @@
     <t>study_id</t>
   </si>
   <si>
-    <t>Chambers_et_al_2020_inland</t>
-  </si>
-  <si>
-    <t>Chambers_et_al_2020_bay</t>
-  </si>
-  <si>
     <t>push core</t>
   </si>
   <si>
@@ -283,7 +277,13 @@
     <t>measured</t>
   </si>
   <si>
-    <t>White_et_al_2019</t>
+    <t>Chambers_et_al_2019</t>
+  </si>
+  <si>
+    <t>White_et_al_2020_a</t>
+  </si>
+  <si>
+    <t>White_et_al_2020_b</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="4" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="I4" s="2">
         <v>384.85</v>
@@ -1421,24 +1421,24 @@
         <v>4</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="I5" s="2">
         <v>384.85</v>
@@ -1450,27 +1450,27 @@
         <v>4</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G6" s="2">
         <v>70</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" s="2">
         <v>550</v>
@@ -1479,16 +1479,16 @@
         <v>3</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating Chambers and White 2020 methods
</commit_message>
<xml_diff>
--- a/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
+++ b/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Chambers_et_al_2019/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453DC003-EBA9-0548-9D7A-039E3D6C7A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA25D48B-B48A-D244-9F68-C68376DDB54F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>coring_method</t>
   </si>
@@ -28,9 +28,6 @@
     <t>roots_flag</t>
   </si>
   <si>
-    <t>sediment_seived_flag</t>
-  </si>
-  <si>
     <t>sediment_sieve_size</t>
   </si>
   <si>
@@ -284,6 +281,24 @@
   </si>
   <si>
     <t>White_et_al_2020_b</t>
+  </si>
+  <si>
+    <t>sediment not sieved</t>
+  </si>
+  <si>
+    <t>roots and rhizomes included</t>
+  </si>
+  <si>
+    <t>not specified</t>
+  </si>
+  <si>
+    <t>core_length_flag</t>
+  </si>
+  <si>
+    <t>core depth limited by length of corer</t>
+  </si>
+  <si>
+    <t>sediment_sieved_flag</t>
   </si>
 </sst>
 </file>
@@ -767,7 +782,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -776,6 +791,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1133,20 +1155,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="31" width="34.5" style="2" customWidth="1"/>
+    <col min="1" max="32" width="34.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1155,341 +1177,445 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:31" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="3" spans="1:31" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="4">
+        <v>70</v>
+      </c>
+      <c r="I4" s="4">
+        <v>72</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="M4" s="4">
+        <v>550</v>
+      </c>
+      <c r="N4" s="4">
+        <v>3</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
     </row>
-    <row r="4" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:32" s="5" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="4">
+        <v>60</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4">
+        <v>384.85</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="4">
+        <v>550</v>
+      </c>
+      <c r="N5" s="4">
+        <v>4</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+    </row>
+    <row r="6" spans="1:32" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="2">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="4">
+        <v>60</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <v>384.85</v>
       </c>
-      <c r="L4" s="2">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="4">
         <v>550</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N6" s="4">
         <v>4</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" s="2" t="b">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="T4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="T6" s="4"/>
+      <c r="U6" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="2">
-        <v>384.85</v>
-      </c>
-      <c r="L5" s="2">
-        <v>550</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="R5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="2">
-        <v>70</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="V6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="2">
-        <v>550</v>
-      </c>
-      <c r="M6" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="R6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Chambers and White data hook and add new col/varname functions to qaqc
</commit_message>
<xml_diff>
--- a/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
+++ b/data/primary_studies/Chambers_et_al_2019/intermediate/Chambers_White_2020_material_and_methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Chambers_et_al_2019/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E3EEE4-A21A-3E4A-A75A-82E6E5B7FA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E864EE6-C0E6-5245-8AE6-29BB2034373E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27000" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>coring_method</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>sediment_sieved_flag</t>
+  </si>
+  <si>
+    <t>no obvious compaction</t>
   </si>
 </sst>
 </file>
@@ -1151,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1427,9 @@
       <c r="A4" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>88</v>
       </c>
@@ -1433,7 +1438,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G4" s="4">
         <v>70</v>
@@ -1494,7 +1499,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G5" s="4">
         <v>60</v>

</xml_diff>